<commit_message>
更新 SC API 完成 DL Last Mile 追踨
</commit_message>
<xml_diff>
--- a/QDLogistics/FileUploads/pickup/Single.xlsx
+++ b/QDLogistics/FileUploads/pickup/Single.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <x:si>
     <x:t>ProductID</x:t>
   </x:si>
@@ -37,10 +37,10 @@
     <x:t>Check</x:t>
   </x:si>
   <x:si>
-    <x:t>106004111</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sony Xperia Z5 Premium E6853 4G LTE (Chrome) (TW)</x:t>
+    <x:t>106003253</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ASUS ZenFone 4 (ZE554KL) 4GB / 64GB (Midnight Black)</x:t>
   </x:si>
   <x:si>
     <x:t>TWN</x:t>
@@ -52,34 +52,52 @@
     <x:t>□</x:t>
   </x:si>
   <x:si>
-    <x:t>106005325</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Samsung GALAXY J2 Prime SM-G532GZ 8GB (Silver)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>106005353</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Samsung Galaxy S8+ (SM-G955F) 64GB (Maple Gold)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>106007173</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LG G6 (H870DS) 64GB (Ice Platinum)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>106018079</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Huawei Nova 2i (RNE-L02) 64GB (Aurora Blue)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>106018085</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Huawei Mate 10 Pro (BLA-L29) 128GB (Midnight Blue)</x:t>
+    <x:t>106003258</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ASUS ZenFone 4 Pro (ZS551KL) 6GB / 64GB (Moonlight White)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>106004166</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sony Xperia XA1 G3125 32GB (Gold)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>106004167</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sony Xperia XA1 G3125 32GB (Pink)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>106005382</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Samsung Galaxy S9 (SM-G960F/DS) 64GB (Coral Blue)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>106006164</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HTC Desire 828 (D828g) 16GB (Pearl White)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>106008063</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nokia 7 Plus (TA-1062) 64GB (White / Copper)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>111008040</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ASUS ZenWatch 3 (WI503Q) (Black)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>111008072</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LG Watch Style W270 (Rose Gold)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -178,8 +196,8 @@
 </file>
 
 <file path=xl/tables/table.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G11" totalsRowShown="0">
-  <x:autoFilter ref="A1:G11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G14" totalsRowShown="0">
+  <x:autoFilter ref="A1:G14"/>
   <x:tableColumns count="7">
     <x:tableColumn id="1" name="ProductID"/>
     <x:tableColumn id="2" name="ProductName"/>
@@ -482,7 +500,7 @@
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
     <x:pageSetUpPr fitToPage="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G11"/>
+  <x:dimension ref="A1:G14"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -533,7 +551,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E2" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F2" s="1" t="s">
         <x:v>10</x:v>
@@ -556,7 +574,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E3" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F3" s="1" t="s">
         <x:v>10</x:v>
@@ -579,7 +597,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F4" s="1" t="s">
         <x:v>10</x:v>
@@ -590,10 +608,10 @@
     </x:row>
     <x:row r="5" spans="1:7">
       <x:c r="A5" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C5" s="1" t="n">
         <x:v>1</x:v>
@@ -602,7 +620,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E5" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F5" s="1" t="s">
         <x:v>10</x:v>
@@ -613,10 +631,10 @@
     </x:row>
     <x:row r="6" spans="1:7">
       <x:c r="A6" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
-        <x:v>19</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C6" s="1" t="n">
         <x:v>1</x:v>
@@ -625,7 +643,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E6" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F6" s="1" t="s">
         <x:v>10</x:v>
@@ -636,10 +654,10 @@
     </x:row>
     <x:row r="7" spans="1:7">
       <x:c r="A7" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B7" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C7" s="1" t="n">
         <x:v>1</x:v>
@@ -648,7 +666,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E7" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F7" s="1" t="s">
         <x:v>10</x:v>
@@ -659,10 +677,10 @@
     </x:row>
     <x:row r="8" spans="1:7">
       <x:c r="A8" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B8" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C8" s="1" t="n">
         <x:v>1</x:v>
@@ -671,7 +689,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E8" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F8" s="1" t="s">
         <x:v>10</x:v>
@@ -682,10 +700,10 @@
     </x:row>
     <x:row r="9" spans="1:7">
       <x:c r="A9" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B9" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C9" s="1" t="n">
         <x:v>1</x:v>
@@ -694,7 +712,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E9" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F9" s="1" t="s">
         <x:v>10</x:v>
@@ -717,7 +735,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E10" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F10" s="1" t="s">
         <x:v>10</x:v>
@@ -728,10 +746,10 @@
     </x:row>
     <x:row r="11" spans="1:7">
       <x:c r="A11" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B11" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C11" s="1" t="n">
         <x:v>1</x:v>
@@ -740,12 +758,81 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E11" s="3">
-        <x:v>43110</x:v>
+        <x:v>43216</x:v>
       </x:c>
       <x:c r="F11" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G11" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:7">
+      <x:c r="A12" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C12" s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D12" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E12" s="3">
+        <x:v>43216</x:v>
+      </x:c>
+      <x:c r="F12" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G12" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:7">
+      <x:c r="A13" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C13" s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D13" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E13" s="3">
+        <x:v>43216</x:v>
+      </x:c>
+      <x:c r="F13" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G13" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:7">
+      <x:c r="A14" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C14" s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D14" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E14" s="3">
+        <x:v>43216</x:v>
+      </x:c>
+      <x:c r="F14" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G14" s="1" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>

</xml_diff>